<commit_message>
New versions matching the code improvements.
</commit_message>
<xml_diff>
--- a/examples/templates/EmploymentContract-Serial.xlsx
+++ b/examples/templates/EmploymentContract-Serial.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D10B8C-D3C8-9A4A-A1FC-14C8F212C6B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5E4FAA-E109-E64E-996A-C97FE18BAA2D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serial" sheetId="4" r:id="rId1"/>
+    <sheet name="Configuration" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Merlin</t>
   </si>
@@ -69,6 +70,44 @@
   <si>
     <t>Here you may define the variables for serial letters.
 For each data row the MS Word® template is used for creating a separate output document.</t>
+  </si>
+  <si>
+    <t>This sheet contains the configuration of this template.
+Please modify this sheet only if you know what you're doing!
+It's recommended to refer the Merlin application for modifying template configurations.</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>TemplateDefinition</t>
+  </si>
+  <si>
+    <t>EmploymentContract-${counter}-${Employee}</t>
+  </si>
+  <si>
+    <t>kjdhe93uuei</t>
+  </si>
+  <si>
+    <t>References a template file by its canonical path, e. g. in the file system.</t>
+  </si>
+  <si>
+    <t>Employment contract</t>
+  </si>
+  <si>
+    <t>FilenamePattern</t>
+  </si>
+  <si>
+    <t>Here you may define the file names of the generated files by this serial function. You can use all Variables of the template as well as the variable ${counter} as a serial number of the file.</t>
   </si>
 </sst>
 </file>
@@ -76,9 +115,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -119,6 +158,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -140,21 +185,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -471,96 +520,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B4FC5B-6DB8-264D-BEB1-6ABB93FD2F3D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5"/>
-    <col min="4" max="4" width="11.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>25</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>40</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>30</v>
       </c>
     </row>
@@ -571,4 +620,88 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE03FD30-3147-A049-AB56-575DB1394E69}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="140.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TemplateDefintion.id isn't a generated value anymore. TemplateDefinition.name is now TemplateDefinition.Id.
</commit_message>
<xml_diff>
--- a/examples/templates/EmploymentContract-Serial.xlsx
+++ b/examples/templates/EmploymentContract-Serial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5E4FAA-E109-E64E-996A-C97FE18BAA2D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F4D898-D2CA-1F48-9ED7-DA10AF6BA30B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serial" sheetId="4" r:id="rId1"/>
@@ -520,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B4FC5B-6DB8-264D-BEB1-6ABB93FD2F3D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE03FD30-3147-A049-AB56-575DB1394E69}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>